<commit_message>
Added all Summary-scenarios except 5
</commit_message>
<xml_diff>
--- a/Code/Limpio/Excels/modelo MM - TALCA 28.12_v6.xlsx
+++ b/Code/Limpio/Excels/modelo MM - TALCA 28.12_v6.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\6020.Inecon_ModeloVanMedicion\6020.Inecon_ModeloVanMedicion\Code\Limpio\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B68758-D6D0-45DC-95DA-037136883ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D44DB40-8FE4-474E-86F9-6B6AE5B27F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="704" activeTab="4" xr2:uid="{0B67A8E0-BE2B-4F48-8F89-95A6B35879D7}"/>
   </bookViews>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="351">
   <si>
     <t>Intervalo (l/h)</t>
   </si>
@@ -1173,16 +1173,10 @@
     <t xml:space="preserve">Capex cercano a </t>
   </si>
   <si>
-    <t>100.000.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Van 0 </t>
-  </si>
-  <si>
-    <t>Número de medidores</t>
-  </si>
-  <si>
     <t>Escenario</t>
+  </si>
+  <si>
+    <t>VAN</t>
   </si>
 </sst>
 </file>
@@ -1663,7 +1657,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="173" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2014,6 +2008,7 @@
     <xf numFmtId="0" fontId="19" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2023,7 +2018,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -11032,7 +11027,7 @@
       <c r="V98" s="75"/>
     </row>
     <row r="99" spans="1:22" s="76" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="158" t="s">
+      <c r="B99" s="159" t="s">
         <v>165</v>
       </c>
       <c r="C99" s="77" t="s">
@@ -11059,7 +11054,7 @@
       <c r="S99" s="78"/>
     </row>
     <row r="100" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B100" s="159"/>
+      <c r="B100" s="160"/>
       <c r="C100" s="79"/>
       <c r="D100" s="80"/>
       <c r="E100" s="80"/>
@@ -11079,7 +11074,7 @@
       <c r="S100" s="80"/>
     </row>
     <row r="101" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B101" s="159"/>
+      <c r="B101" s="160"/>
       <c r="C101" s="76" t="s">
         <v>167</v>
       </c>
@@ -11104,7 +11099,7 @@
       <c r="S101" s="80"/>
     </row>
     <row r="102" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B102" s="159"/>
+      <c r="B102" s="160"/>
       <c r="D102" s="81"/>
       <c r="E102" s="81"/>
       <c r="F102" s="81"/>
@@ -11123,7 +11118,7 @@
       <c r="S102" s="81"/>
     </row>
     <row r="103" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B103" s="159"/>
+      <c r="B103" s="160"/>
       <c r="D103" s="81"/>
       <c r="E103" s="81"/>
       <c r="F103" s="81"/>
@@ -11142,7 +11137,7 @@
       <c r="S103" s="81"/>
     </row>
     <row r="104" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B104" s="159"/>
+      <c r="B104" s="160"/>
       <c r="C104" s="79" t="s">
         <v>168</v>
       </c>
@@ -11213,7 +11208,7 @@
       <c r="A105" s="76">
         <v>1</v>
       </c>
-      <c r="B105" s="159"/>
+      <c r="B105" s="160"/>
       <c r="C105" s="76" t="s">
         <v>169</v>
       </c>
@@ -11281,7 +11276,7 @@
       <c r="U105" s="82"/>
     </row>
     <row r="106" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B106" s="159"/>
+      <c r="B106" s="160"/>
       <c r="C106" s="83"/>
       <c r="D106" s="84"/>
       <c r="E106" s="85"/>
@@ -11301,7 +11296,7 @@
       <c r="S106" s="85"/>
     </row>
     <row r="107" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B107" s="159"/>
+      <c r="B107" s="160"/>
       <c r="C107" s="76" t="s">
         <v>170</v>
       </c>
@@ -11323,7 +11318,7 @@
       <c r="S107" s="81"/>
     </row>
     <row r="108" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B108" s="159"/>
+      <c r="B108" s="160"/>
       <c r="C108" s="86" t="s">
         <v>171</v>
       </c>
@@ -11349,7 +11344,7 @@
       <c r="T108" s="87"/>
     </row>
     <row r="109" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B109" s="159"/>
+      <c r="B109" s="160"/>
       <c r="C109" s="86" t="s">
         <v>172</v>
       </c>
@@ -11420,7 +11415,7 @@
       <c r="A110" s="76">
         <v>10</v>
       </c>
-      <c r="B110" s="159"/>
+      <c r="B110" s="160"/>
       <c r="C110" s="86" t="s">
         <v>173</v>
       </c>
@@ -11490,7 +11485,7 @@
       <c r="A111" s="88">
         <v>0.27</v>
       </c>
-      <c r="B111" s="160"/>
+      <c r="B111" s="161"/>
       <c r="C111" s="89" t="s">
         <v>174</v>
       </c>
@@ -17500,7 +17495,7 @@
       <c r="V99" s="75"/>
     </row>
     <row r="100" spans="1:22" s="76" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="158" t="s">
+      <c r="B100" s="159" t="s">
         <v>165</v>
       </c>
       <c r="C100" s="77" t="s">
@@ -17527,7 +17522,7 @@
       <c r="S100" s="78"/>
     </row>
     <row r="101" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B101" s="159"/>
+      <c r="B101" s="160"/>
       <c r="C101" s="79"/>
       <c r="D101" s="80"/>
       <c r="E101" s="80"/>
@@ -17547,7 +17542,7 @@
       <c r="S101" s="80"/>
     </row>
     <row r="102" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B102" s="159"/>
+      <c r="B102" s="160"/>
       <c r="C102" s="76" t="s">
         <v>167</v>
       </c>
@@ -17572,7 +17567,7 @@
       <c r="S102" s="80"/>
     </row>
     <row r="103" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B103" s="159"/>
+      <c r="B103" s="160"/>
       <c r="D103" s="81"/>
       <c r="E103" s="81"/>
       <c r="F103" s="81"/>
@@ -17591,7 +17586,7 @@
       <c r="S103" s="81"/>
     </row>
     <row r="104" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B104" s="159"/>
+      <c r="B104" s="160"/>
       <c r="D104" s="81"/>
       <c r="E104" s="81"/>
       <c r="F104" s="81"/>
@@ -17610,7 +17605,7 @@
       <c r="S104" s="81"/>
     </row>
     <row r="105" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B105" s="159"/>
+      <c r="B105" s="160"/>
       <c r="C105" s="79" t="s">
         <v>168</v>
       </c>
@@ -17681,7 +17676,7 @@
       <c r="A106" s="76">
         <v>1</v>
       </c>
-      <c r="B106" s="159"/>
+      <c r="B106" s="160"/>
       <c r="C106" s="76" t="s">
         <v>169</v>
       </c>
@@ -17749,7 +17744,7 @@
       <c r="U106" s="82"/>
     </row>
     <row r="107" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B107" s="159"/>
+      <c r="B107" s="160"/>
       <c r="C107" s="83"/>
       <c r="D107" s="84"/>
       <c r="E107" s="85"/>
@@ -17769,7 +17764,7 @@
       <c r="S107" s="85"/>
     </row>
     <row r="108" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B108" s="159"/>
+      <c r="B108" s="160"/>
       <c r="C108" s="76" t="s">
         <v>170</v>
       </c>
@@ -17791,7 +17786,7 @@
       <c r="S108" s="81"/>
     </row>
     <row r="109" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B109" s="159"/>
+      <c r="B109" s="160"/>
       <c r="C109" s="86" t="s">
         <v>171</v>
       </c>
@@ -17817,7 +17812,7 @@
       <c r="T109" s="87"/>
     </row>
     <row r="110" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B110" s="159"/>
+      <c r="B110" s="160"/>
       <c r="C110" s="86" t="s">
         <v>172</v>
       </c>
@@ -17888,7 +17883,7 @@
       <c r="A111" s="76">
         <v>10</v>
       </c>
-      <c r="B111" s="159"/>
+      <c r="B111" s="160"/>
       <c r="C111" s="86" t="s">
         <v>173</v>
       </c>
@@ -17958,7 +17953,7 @@
       <c r="A112" s="88">
         <v>0.27</v>
       </c>
-      <c r="B112" s="160"/>
+      <c r="B112" s="161"/>
       <c r="C112" s="89" t="s">
         <v>174</v>
       </c>
@@ -21784,7 +21779,7 @@
       <c r="V50" s="75"/>
     </row>
     <row r="51" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="158" t="s">
+      <c r="B51" s="159" t="s">
         <v>165</v>
       </c>
       <c r="C51" s="77" t="s">
@@ -21842,7 +21837,7 @@
       </c>
     </row>
     <row r="52" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="159"/>
+      <c r="B52" s="160"/>
       <c r="C52" s="79"/>
       <c r="D52" s="80"/>
       <c r="E52" s="80"/>
@@ -21862,7 +21857,7 @@
       <c r="S52" s="80"/>
     </row>
     <row r="53" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="159"/>
+      <c r="B53" s="160"/>
       <c r="C53" s="76" t="s">
         <v>167</v>
       </c>
@@ -21884,7 +21879,7 @@
       <c r="S53" s="80"/>
     </row>
     <row r="54" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="159"/>
+      <c r="B54" s="160"/>
       <c r="D54" s="81"/>
       <c r="E54" s="81"/>
       <c r="F54" s="81"/>
@@ -21903,7 +21898,7 @@
       <c r="S54" s="81"/>
     </row>
     <row r="55" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="159"/>
+      <c r="B55" s="160"/>
       <c r="D55" s="81"/>
       <c r="E55" s="81"/>
       <c r="F55" s="81"/>
@@ -21922,7 +21917,7 @@
       <c r="S55" s="81"/>
     </row>
     <row r="56" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="159"/>
+      <c r="B56" s="160"/>
       <c r="C56" s="79" t="s">
         <v>168</v>
       </c>
@@ -21992,7 +21987,7 @@
       <c r="A57" s="76">
         <v>1</v>
       </c>
-      <c r="B57" s="159"/>
+      <c r="B57" s="160"/>
       <c r="C57" s="76" t="s">
         <v>169</v>
       </c>
@@ -22059,7 +22054,7 @@
       </c>
     </row>
     <row r="58" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="159"/>
+      <c r="B58" s="160"/>
       <c r="C58" s="83"/>
       <c r="D58" s="84"/>
       <c r="E58" s="85"/>
@@ -22079,7 +22074,7 @@
       <c r="S58" s="85"/>
     </row>
     <row r="59" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="159"/>
+      <c r="B59" s="160"/>
       <c r="C59" s="76" t="s">
         <v>170</v>
       </c>
@@ -22101,7 +22096,7 @@
       <c r="S59" s="81"/>
     </row>
     <row r="60" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="159"/>
+      <c r="B60" s="160"/>
       <c r="C60" s="86" t="s">
         <v>171</v>
       </c>
@@ -22129,7 +22124,7 @@
       <c r="A61" s="76">
         <v>10</v>
       </c>
-      <c r="B61" s="159"/>
+      <c r="B61" s="160"/>
       <c r="C61" s="86" t="s">
         <v>173</v>
       </c>
@@ -22199,7 +22194,7 @@
       <c r="A62" s="88">
         <v>0.27</v>
       </c>
-      <c r="B62" s="160"/>
+      <c r="B62" s="161"/>
       <c r="C62" s="89" t="s">
         <v>174</v>
       </c>
@@ -24640,18 +24635,18 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="127" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B1" s="127" t="s">
         <v>336</v>
@@ -24665,9 +24660,9 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>351</v>
-      </c>
-      <c r="C2" s="161">
+        <v>350</v>
+      </c>
+      <c r="C2" s="158">
         <v>1</v>
       </c>
     </row>
@@ -24689,8 +24684,8 @@
       <c r="B4" t="s">
         <v>347</v>
       </c>
-      <c r="C4" s="22">
-        <v>0.3</v>
+      <c r="C4" s="162">
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -24700,8 +24695,8 @@
       <c r="B5" t="s">
         <v>348</v>
       </c>
-      <c r="C5" t="s">
-        <v>349</v>
+      <c r="C5">
+        <v>600000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -24709,7 +24704,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>350</v>
+        <v>180</v>
       </c>
       <c r="C6" s="153">
         <v>7.0000000000000007E-2</v>
@@ -28947,11 +28942,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="afef9374-bd24-49fe-b5be-cd056ccbd7a9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29143,26 +29139,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="afef9374-bd24-49fe-b5be-cd056ccbd7a9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F368767-011F-4603-B6D3-67B09FEB0E3E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{799D9F8D-2034-4116-9680-A411761E28F5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="afef9374-bd24-49fe-b5be-cd056ccbd7a9"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -29186,9 +29173,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{799D9F8D-2034-4116-9680-A411761E28F5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F368767-011F-4603-B6D3-67B09FEB0E3E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="afef9374-bd24-49fe-b5be-cd056ccbd7a9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Funcionando el cambio (excepto IyF)
</commit_message>
<xml_diff>
--- a/Code/Limpio/Excels/modelo MM - TALCA 28.12_v6.xlsx
+++ b/Code/Limpio/Excels/modelo MM - TALCA 28.12_v6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\6020.Inecon_ModeloVanMedicion\6020.Inecon_ModeloVanMedicion\Code\Limpio\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C01350-A12D-4D9D-9360-2C7C25F021E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918D23C9-5D7A-4A4D-AE46-34884BA73132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="704" activeTab="4" xr2:uid="{0B67A8E0-BE2B-4F48-8F89-95A6B35879D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="834" firstSheet="7" activeTab="13" xr2:uid="{0B67A8E0-BE2B-4F48-8F89-95A6B35879D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos_Tarifas" sheetId="13" r:id="rId1"/>
@@ -26,14 +26,16 @@
     <sheet name="EDAD" sheetId="2" r:id="rId11"/>
     <sheet name="PROGRAMA AUTOCONTROL" sheetId="5" r:id="rId12"/>
     <sheet name="CLASES" sheetId="3" r:id="rId13"/>
-    <sheet name="REFERENCIA CLASES DECAIMIENTO" sheetId="10" r:id="rId14"/>
-    <sheet name="CAUDAL ORIGINAL" sheetId="1" r:id="rId15"/>
+    <sheet name="REFERENCIA DECAIMIENTO" sheetId="19" r:id="rId14"/>
+    <sheet name="REFERENCIA CLASES DECAIMIENTO" sheetId="10" r:id="rId15"/>
+    <sheet name="CAUDAL ORIGINAL" sheetId="1" r:id="rId16"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId16"/>
+    <externalReference r:id="rId17"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">DATOS!$A$1:$G$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'REFERENCIA DECAIMIENTO'!$A$1:$B$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -124,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="355">
   <si>
     <t>Intervalo (l/h)</t>
   </si>
@@ -1177,6 +1179,18 @@
   </si>
   <si>
     <t>VAN</t>
+  </si>
+  <si>
+    <t>Referencia Decaimiento Base</t>
+  </si>
+  <si>
+    <t>Referencia Decaimiento Reemplazo</t>
+  </si>
+  <si>
+    <t>CLASE_BASE</t>
+  </si>
+  <si>
+    <t>DIAMETRO_MEDIDOR_BASE</t>
   </si>
 </sst>
 </file>
@@ -1336,7 +1350,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1424,6 +1438,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1657,7 +1677,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="173" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2010,6 +2030,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2029,7 +2052,14 @@
     <cellStyle name="Normal 2" xfId="3" xr:uid="{95AB7D82-70C6-4489-B31A-733E3E846161}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4440,7 +4470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF05CA6D-B359-469D-BCFA-0D1A2EFC1F75}">
   <dimension ref="A1:F170"/>
   <sheetViews>
-    <sheetView topLeftCell="A151" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
@@ -7104,7 +7134,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7223,11 +7253,682 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CBA8B56-86C0-48DC-8876-01FB76341A5D}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" style="32" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="32"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="160" t="s">
+        <v>353</v>
+      </c>
+      <c r="B1" s="160" t="s">
+        <v>354</v>
+      </c>
+      <c r="C1" s="160" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1" s="160" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="31">
+        <v>13</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="31" t="str">
+        <f t="shared" ref="D2:D43" si="0">IF(B2&lt;=25, "C-"&amp;B2, "ULTRA")</f>
+        <v>C-13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="31">
+        <v>19</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="31">
+        <v>25</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="31">
+        <v>38</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="31">
+        <v>50</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="31">
+        <v>13</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="31">
+        <v>19</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="31">
+        <v>25</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="31">
+        <v>32</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="31">
+        <v>38</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="31">
+        <v>50</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="31">
+        <v>75</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="31">
+        <v>80</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="31">
+        <v>100</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="31">
+        <v>13</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="31">
+        <v>19</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="31">
+        <v>25</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="31">
+        <v>38</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="31">
+        <v>50</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="31">
+        <v>80</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="31">
+        <v>13</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="31">
+        <v>19</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="31">
+        <v>25</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="31">
+        <v>38</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="31">
+        <v>13</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="31">
+        <v>19</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="31">
+        <v>25</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="31">
+        <v>50</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="31">
+        <v>80</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="31">
+        <v>13</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="31">
+        <v>19</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="31">
+        <v>13</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="31">
+        <v>19</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="31">
+        <v>25</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="31">
+        <v>13</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="31">
+        <v>19</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="31">
+        <v>50</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="31">
+        <v>80</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="31">
+        <v>13</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="31">
+        <v>19</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="31">
+        <v>25</v>
+      </c>
+      <c r="C42" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>C-25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="31">
+        <v>38</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="31" t="str">
+        <f t="shared" si="0"/>
+        <v>ULTRA</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B43" xr:uid="{1ADB41F7-39CC-43DC-8921-627CB556F46F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B43">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACB5FF1-7A28-46AB-AC06-FB476C488476}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7298,12 +7999,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9D5E7F-12B8-4A53-9E8A-63ABDC168AAE}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11027,7 +11728,7 @@
       <c r="V98" s="75"/>
     </row>
     <row r="99" spans="1:22" s="76" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="160" t="s">
+      <c r="B99" s="161" t="s">
         <v>165</v>
       </c>
       <c r="C99" s="77" t="s">
@@ -11054,7 +11755,7 @@
       <c r="S99" s="78"/>
     </row>
     <row r="100" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B100" s="161"/>
+      <c r="B100" s="162"/>
       <c r="C100" s="79"/>
       <c r="D100" s="80"/>
       <c r="E100" s="80"/>
@@ -11074,7 +11775,7 @@
       <c r="S100" s="80"/>
     </row>
     <row r="101" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B101" s="161"/>
+      <c r="B101" s="162"/>
       <c r="C101" s="76" t="s">
         <v>167</v>
       </c>
@@ -11099,7 +11800,7 @@
       <c r="S101" s="80"/>
     </row>
     <row r="102" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B102" s="161"/>
+      <c r="B102" s="162"/>
       <c r="D102" s="81"/>
       <c r="E102" s="81"/>
       <c r="F102" s="81"/>
@@ -11118,7 +11819,7 @@
       <c r="S102" s="81"/>
     </row>
     <row r="103" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B103" s="161"/>
+      <c r="B103" s="162"/>
       <c r="D103" s="81"/>
       <c r="E103" s="81"/>
       <c r="F103" s="81"/>
@@ -11137,7 +11838,7 @@
       <c r="S103" s="81"/>
     </row>
     <row r="104" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B104" s="161"/>
+      <c r="B104" s="162"/>
       <c r="C104" s="79" t="s">
         <v>168</v>
       </c>
@@ -11208,7 +11909,7 @@
       <c r="A105" s="76">
         <v>1</v>
       </c>
-      <c r="B105" s="161"/>
+      <c r="B105" s="162"/>
       <c r="C105" s="76" t="s">
         <v>169</v>
       </c>
@@ -11276,7 +11977,7 @@
       <c r="U105" s="82"/>
     </row>
     <row r="106" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B106" s="161"/>
+      <c r="B106" s="162"/>
       <c r="C106" s="83"/>
       <c r="D106" s="84"/>
       <c r="E106" s="85"/>
@@ -11296,7 +11997,7 @@
       <c r="S106" s="85"/>
     </row>
     <row r="107" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B107" s="161"/>
+      <c r="B107" s="162"/>
       <c r="C107" s="76" t="s">
         <v>170</v>
       </c>
@@ -11318,7 +12019,7 @@
       <c r="S107" s="81"/>
     </row>
     <row r="108" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B108" s="161"/>
+      <c r="B108" s="162"/>
       <c r="C108" s="86" t="s">
         <v>171</v>
       </c>
@@ -11344,7 +12045,7 @@
       <c r="T108" s="87"/>
     </row>
     <row r="109" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B109" s="161"/>
+      <c r="B109" s="162"/>
       <c r="C109" s="86" t="s">
         <v>172</v>
       </c>
@@ -11415,7 +12116,7 @@
       <c r="A110" s="76">
         <v>10</v>
       </c>
-      <c r="B110" s="161"/>
+      <c r="B110" s="162"/>
       <c r="C110" s="86" t="s">
         <v>173</v>
       </c>
@@ -11485,7 +12186,7 @@
       <c r="A111" s="88">
         <v>0.27</v>
       </c>
-      <c r="B111" s="162"/>
+      <c r="B111" s="163"/>
       <c r="C111" s="89" t="s">
         <v>174</v>
       </c>
@@ -17495,7 +18196,7 @@
       <c r="V99" s="75"/>
     </row>
     <row r="100" spans="1:22" s="76" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="160" t="s">
+      <c r="B100" s="161" t="s">
         <v>165</v>
       </c>
       <c r="C100" s="77" t="s">
@@ -17522,7 +18223,7 @@
       <c r="S100" s="78"/>
     </row>
     <row r="101" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B101" s="161"/>
+      <c r="B101" s="162"/>
       <c r="C101" s="79"/>
       <c r="D101" s="80"/>
       <c r="E101" s="80"/>
@@ -17542,7 +18243,7 @@
       <c r="S101" s="80"/>
     </row>
     <row r="102" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B102" s="161"/>
+      <c r="B102" s="162"/>
       <c r="C102" s="76" t="s">
         <v>167</v>
       </c>
@@ -17567,7 +18268,7 @@
       <c r="S102" s="80"/>
     </row>
     <row r="103" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B103" s="161"/>
+      <c r="B103" s="162"/>
       <c r="D103" s="81"/>
       <c r="E103" s="81"/>
       <c r="F103" s="81"/>
@@ -17586,7 +18287,7 @@
       <c r="S103" s="81"/>
     </row>
     <row r="104" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B104" s="161"/>
+      <c r="B104" s="162"/>
       <c r="D104" s="81"/>
       <c r="E104" s="81"/>
       <c r="F104" s="81"/>
@@ -17605,7 +18306,7 @@
       <c r="S104" s="81"/>
     </row>
     <row r="105" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B105" s="161"/>
+      <c r="B105" s="162"/>
       <c r="C105" s="79" t="s">
         <v>168</v>
       </c>
@@ -17676,7 +18377,7 @@
       <c r="A106" s="76">
         <v>1</v>
       </c>
-      <c r="B106" s="161"/>
+      <c r="B106" s="162"/>
       <c r="C106" s="76" t="s">
         <v>169</v>
       </c>
@@ -17744,7 +18445,7 @@
       <c r="U106" s="82"/>
     </row>
     <row r="107" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B107" s="161"/>
+      <c r="B107" s="162"/>
       <c r="C107" s="83"/>
       <c r="D107" s="84"/>
       <c r="E107" s="85"/>
@@ -17764,7 +18465,7 @@
       <c r="S107" s="85"/>
     </row>
     <row r="108" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B108" s="161"/>
+      <c r="B108" s="162"/>
       <c r="C108" s="76" t="s">
         <v>170</v>
       </c>
@@ -17786,7 +18487,7 @@
       <c r="S108" s="81"/>
     </row>
     <row r="109" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B109" s="161"/>
+      <c r="B109" s="162"/>
       <c r="C109" s="86" t="s">
         <v>171</v>
       </c>
@@ -17812,7 +18513,7 @@
       <c r="T109" s="87"/>
     </row>
     <row r="110" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B110" s="161"/>
+      <c r="B110" s="162"/>
       <c r="C110" s="86" t="s">
         <v>172</v>
       </c>
@@ -17883,7 +18584,7 @@
       <c r="A111" s="76">
         <v>10</v>
       </c>
-      <c r="B111" s="161"/>
+      <c r="B111" s="162"/>
       <c r="C111" s="86" t="s">
         <v>173</v>
       </c>
@@ -17953,7 +18654,7 @@
       <c r="A112" s="88">
         <v>0.27</v>
       </c>
-      <c r="B112" s="162"/>
+      <c r="B112" s="163"/>
       <c r="C112" s="89" t="s">
         <v>174</v>
       </c>
@@ -21779,7 +22480,7 @@
       <c r="V50" s="75"/>
     </row>
     <row r="51" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="160" t="s">
+      <c r="B51" s="161" t="s">
         <v>165</v>
       </c>
       <c r="C51" s="77" t="s">
@@ -21837,7 +22538,7 @@
       </c>
     </row>
     <row r="52" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="161"/>
+      <c r="B52" s="162"/>
       <c r="C52" s="79"/>
       <c r="D52" s="80"/>
       <c r="E52" s="80"/>
@@ -21857,7 +22558,7 @@
       <c r="S52" s="80"/>
     </row>
     <row r="53" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="161"/>
+      <c r="B53" s="162"/>
       <c r="C53" s="76" t="s">
         <v>167</v>
       </c>
@@ -21879,7 +22580,7 @@
       <c r="S53" s="80"/>
     </row>
     <row r="54" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="161"/>
+      <c r="B54" s="162"/>
       <c r="D54" s="81"/>
       <c r="E54" s="81"/>
       <c r="F54" s="81"/>
@@ -21898,7 +22599,7 @@
       <c r="S54" s="81"/>
     </row>
     <row r="55" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="161"/>
+      <c r="B55" s="162"/>
       <c r="D55" s="81"/>
       <c r="E55" s="81"/>
       <c r="F55" s="81"/>
@@ -21917,7 +22618,7 @@
       <c r="S55" s="81"/>
     </row>
     <row r="56" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="161"/>
+      <c r="B56" s="162"/>
       <c r="C56" s="79" t="s">
         <v>168</v>
       </c>
@@ -21987,7 +22688,7 @@
       <c r="A57" s="76">
         <v>1</v>
       </c>
-      <c r="B57" s="161"/>
+      <c r="B57" s="162"/>
       <c r="C57" s="76" t="s">
         <v>169</v>
       </c>
@@ -22054,7 +22755,7 @@
       </c>
     </row>
     <row r="58" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="161"/>
+      <c r="B58" s="162"/>
       <c r="C58" s="83"/>
       <c r="D58" s="84"/>
       <c r="E58" s="85"/>
@@ -22074,7 +22775,7 @@
       <c r="S58" s="85"/>
     </row>
     <row r="59" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="161"/>
+      <c r="B59" s="162"/>
       <c r="C59" s="76" t="s">
         <v>170</v>
       </c>
@@ -22096,7 +22797,7 @@
       <c r="S59" s="81"/>
     </row>
     <row r="60" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="161"/>
+      <c r="B60" s="162"/>
       <c r="C60" s="86" t="s">
         <v>171</v>
       </c>
@@ -22124,7 +22825,7 @@
       <c r="A61" s="76">
         <v>10</v>
       </c>
-      <c r="B61" s="161"/>
+      <c r="B61" s="162"/>
       <c r="C61" s="86" t="s">
         <v>173</v>
       </c>
@@ -22194,7 +22895,7 @@
       <c r="A62" s="88">
         <v>0.27</v>
       </c>
-      <c r="B62" s="162"/>
+      <c r="B62" s="163"/>
       <c r="C62" s="89" t="s">
         <v>174</v>
       </c>
@@ -24634,7 +25335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE05537-58FE-4961-80AD-B200345AF076}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -27660,7 +28361,7 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27722,7 +28423,7 @@
         <v>13</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G8" si="0">A2</f>
+        <f t="shared" ref="G2:G61" si="0">A2</f>
         <v>CAUQUENES</v>
       </c>
       <c r="I2" s="151" t="s">
@@ -27892,409 +28593,1282 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="151"/>
-      <c r="B9" s="151"/>
-      <c r="C9" s="154"/>
-      <c r="D9" s="151"/>
-      <c r="E9" s="151"/>
-      <c r="F9" s="151"/>
+      <c r="A9" s="151" t="s">
+        <v>228</v>
+      </c>
+      <c r="B9" s="151">
+        <v>38</v>
+      </c>
+      <c r="C9" s="154">
+        <v>42815</v>
+      </c>
+      <c r="D9" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="151">
+        <v>1244544</v>
+      </c>
+      <c r="F9" s="151">
+        <v>50</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>CONSTITUCION</v>
+      </c>
       <c r="I9" s="151" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="151"/>
-      <c r="B10" s="151"/>
-      <c r="C10" s="154"/>
-      <c r="D10" s="151"/>
-      <c r="E10" s="151"/>
-      <c r="F10" s="151"/>
+      <c r="A10" s="151" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" s="151">
+        <v>38</v>
+      </c>
+      <c r="C10" s="154">
+        <v>40256</v>
+      </c>
+      <c r="D10" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="151">
+        <v>696717</v>
+      </c>
+      <c r="F10" s="151">
+        <v>31</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>CONSTITUCION</v>
+      </c>
       <c r="I10" s="151" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="151"/>
-      <c r="B11" s="151"/>
-      <c r="C11" s="154"/>
-      <c r="D11" s="151"/>
-      <c r="E11" s="151"/>
-      <c r="F11" s="151"/>
+      <c r="A11" s="151" t="s">
+        <v>228</v>
+      </c>
+      <c r="B11" s="151">
+        <v>38</v>
+      </c>
+      <c r="C11" s="154">
+        <v>43467</v>
+      </c>
+      <c r="D11" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="151">
+        <v>294987</v>
+      </c>
+      <c r="F11" s="151">
+        <v>44</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>CONSTITUCION</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="151"/>
-      <c r="B12" s="151"/>
-      <c r="C12" s="154"/>
-      <c r="D12" s="151"/>
-      <c r="E12" s="151"/>
-      <c r="F12" s="151"/>
+      <c r="A12" s="151" t="s">
+        <v>228</v>
+      </c>
+      <c r="B12" s="151">
+        <v>38</v>
+      </c>
+      <c r="C12" s="154">
+        <v>41744</v>
+      </c>
+      <c r="D12" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="151">
+        <v>942361</v>
+      </c>
+      <c r="F12" s="151">
+        <v>275</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>CONSTITUCION</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F13" s="151"/>
+      <c r="A13" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13">
+        <v>38</v>
+      </c>
+      <c r="C13" s="38">
+        <v>42167</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13">
+        <v>4299684</v>
+      </c>
+      <c r="F13" s="151">
+        <v>56</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>CONSTITUCION</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F14" s="151"/>
+      <c r="A14" t="s">
+        <v>228</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14" s="38">
+        <v>43420</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14">
+        <v>60219892</v>
+      </c>
+      <c r="F14" s="151">
+        <v>774</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>CONSTITUCION</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F15" s="151"/>
+      <c r="A15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B15">
+        <v>50</v>
+      </c>
+      <c r="C15" s="38">
+        <v>43294</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15">
+        <v>60091707</v>
+      </c>
+      <c r="F15" s="151">
+        <v>178</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>CONSTITUCION</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="151"/>
-      <c r="B16" s="151"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="151"/>
-      <c r="E16" s="151"/>
-      <c r="F16" s="151"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F17" s="151"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F18" s="151"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="151"/>
-      <c r="B19" s="151"/>
-      <c r="C19" s="154"/>
-      <c r="D19" s="151"/>
-      <c r="E19" s="151"/>
-      <c r="F19" s="151"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="151"/>
-      <c r="B20" s="151"/>
-      <c r="C20" s="154"/>
-      <c r="D20" s="151"/>
-      <c r="E20" s="151"/>
-      <c r="F20" s="151"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="151"/>
-      <c r="B21" s="151"/>
-      <c r="C21" s="154"/>
-      <c r="D21" s="151"/>
-      <c r="E21" s="151"/>
-      <c r="F21" s="151"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="151"/>
-      <c r="B22" s="151"/>
-      <c r="C22" s="154"/>
-      <c r="D22" s="151"/>
-      <c r="E22" s="151"/>
-      <c r="F22" s="151"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="151"/>
-      <c r="B23" s="151"/>
-      <c r="C23" s="154"/>
-      <c r="D23" s="151"/>
-      <c r="E23" s="151"/>
-      <c r="F23" s="151"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="151"/>
-      <c r="B24" s="151"/>
-      <c r="C24" s="154"/>
-      <c r="D24" s="151"/>
-      <c r="E24" s="151"/>
-      <c r="F24" s="151"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="151"/>
-      <c r="B25" s="151"/>
-      <c r="C25" s="154"/>
-      <c r="D25" s="151"/>
-      <c r="E25" s="151"/>
-      <c r="F25" s="151"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="151"/>
-      <c r="B26" s="151"/>
-      <c r="C26" s="154"/>
-      <c r="D26" s="151"/>
-      <c r="E26" s="151"/>
-      <c r="F26" s="151"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="151"/>
-      <c r="B27" s="151"/>
-      <c r="C27" s="154"/>
-      <c r="D27" s="151"/>
-      <c r="E27" s="151"/>
-      <c r="F27" s="151"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="151"/>
-      <c r="B28" s="151"/>
-      <c r="C28" s="154"/>
-      <c r="D28" s="151"/>
-      <c r="E28" s="151"/>
-      <c r="F28" s="151"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="151"/>
-      <c r="B29" s="151"/>
-      <c r="C29" s="154"/>
-      <c r="D29" s="151"/>
-      <c r="E29" s="151"/>
-      <c r="F29" s="151"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="151"/>
-      <c r="B30" s="151"/>
-      <c r="C30" s="154"/>
-      <c r="D30" s="151"/>
-      <c r="E30" s="151"/>
-      <c r="F30" s="151"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="151"/>
-      <c r="B31" s="151"/>
-      <c r="C31" s="154"/>
-      <c r="D31" s="151"/>
-      <c r="E31" s="151"/>
-      <c r="F31" s="151"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="151"/>
-      <c r="B32" s="151"/>
-      <c r="C32" s="154"/>
-      <c r="D32" s="151"/>
-      <c r="E32" s="151"/>
-      <c r="F32" s="151"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="151"/>
-      <c r="B33" s="151"/>
-      <c r="C33" s="154"/>
-      <c r="D33" s="151"/>
-      <c r="E33" s="151"/>
-      <c r="F33" s="151"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="151"/>
-      <c r="B34" s="151"/>
-      <c r="C34" s="154"/>
-      <c r="D34" s="151"/>
-      <c r="E34" s="151"/>
-      <c r="F34" s="151"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="151"/>
-      <c r="B35" s="151"/>
-      <c r="C35" s="154"/>
-      <c r="D35" s="151"/>
-      <c r="E35" s="151"/>
-      <c r="F35" s="151"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="151"/>
-      <c r="B36" s="151"/>
-      <c r="C36" s="154"/>
-      <c r="D36" s="151"/>
-      <c r="E36" s="151"/>
-      <c r="F36" s="151"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="151"/>
-      <c r="B37" s="151"/>
-      <c r="C37" s="154"/>
-      <c r="D37" s="151"/>
-      <c r="E37" s="151"/>
-      <c r="F37" s="151"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="151"/>
-      <c r="B38" s="151"/>
-      <c r="C38" s="154"/>
-      <c r="D38" s="151"/>
-      <c r="E38" s="151"/>
-      <c r="F38" s="151"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="151"/>
-      <c r="B39" s="151"/>
-      <c r="C39" s="154"/>
-      <c r="D39" s="151"/>
-      <c r="E39" s="151"/>
-      <c r="F39" s="151"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="151"/>
-      <c r="B40" s="151"/>
-      <c r="C40" s="154"/>
-      <c r="D40" s="151"/>
-      <c r="E40" s="151"/>
-      <c r="F40" s="151"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="151"/>
-      <c r="B41" s="151"/>
-      <c r="C41" s="154"/>
-      <c r="D41" s="151"/>
-      <c r="E41" s="151"/>
-      <c r="F41" s="151"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="151"/>
-      <c r="B42" s="151"/>
-      <c r="C42" s="154"/>
-      <c r="D42" s="151"/>
-      <c r="E42" s="151"/>
-      <c r="F42" s="151"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="151"/>
-      <c r="B43" s="151"/>
-      <c r="C43" s="154"/>
-      <c r="D43" s="151"/>
-      <c r="E43" s="151"/>
-      <c r="F43" s="151"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="151"/>
-      <c r="B44" s="151"/>
-      <c r="C44" s="154"/>
-      <c r="D44" s="151"/>
-      <c r="E44" s="151"/>
-      <c r="F44" s="151"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="151"/>
-      <c r="B45" s="151"/>
-      <c r="C45" s="154"/>
-      <c r="D45" s="151"/>
-      <c r="E45" s="151"/>
-      <c r="F45" s="151"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="151"/>
-      <c r="B46" s="151"/>
-      <c r="C46" s="154"/>
-      <c r="D46" s="151"/>
-      <c r="E46" s="151"/>
-      <c r="F46" s="151"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="151"/>
-      <c r="B47" s="151"/>
-      <c r="C47" s="154"/>
-      <c r="D47" s="151"/>
-      <c r="E47" s="151"/>
-      <c r="F47" s="151"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="151"/>
-      <c r="B48" s="151"/>
-      <c r="C48" s="154"/>
-      <c r="D48" s="151"/>
-      <c r="E48" s="151"/>
-      <c r="F48" s="151"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="151"/>
-      <c r="B49" s="151"/>
-      <c r="C49" s="154"/>
-      <c r="D49" s="151"/>
-      <c r="E49" s="151"/>
-      <c r="F49" s="151"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="151"/>
-      <c r="B50" s="151"/>
-      <c r="C50" s="154"/>
-      <c r="D50" s="151"/>
-      <c r="E50" s="151"/>
-      <c r="F50" s="151"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="151"/>
-      <c r="B51" s="151"/>
-      <c r="C51" s="154"/>
-      <c r="D51" s="151"/>
-      <c r="E51" s="151"/>
-      <c r="F51" s="151"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="151"/>
-      <c r="B52" s="151"/>
-      <c r="C52" s="154"/>
-      <c r="D52" s="151"/>
-      <c r="E52" s="151"/>
-      <c r="F52" s="151"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="151"/>
-      <c r="B53" s="151"/>
-      <c r="C53" s="154"/>
-      <c r="D53" s="151"/>
-      <c r="E53" s="151"/>
-      <c r="F53" s="151"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="151"/>
-      <c r="B54" s="151"/>
-      <c r="C54" s="154"/>
-      <c r="D54" s="151"/>
-      <c r="E54" s="151"/>
-      <c r="F54" s="151"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="151"/>
-      <c r="B55" s="151"/>
-      <c r="C55" s="154"/>
-      <c r="D55" s="151"/>
-      <c r="E55" s="151"/>
-      <c r="F55" s="151"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="151"/>
-      <c r="B56" s="151"/>
-      <c r="C56" s="154"/>
-      <c r="D56" s="151"/>
-      <c r="E56" s="151"/>
-      <c r="F56" s="151"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="151"/>
-      <c r="B57" s="151"/>
-      <c r="C57" s="154"/>
-      <c r="D57" s="151"/>
-      <c r="E57" s="151"/>
-      <c r="F57" s="151"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="151"/>
-      <c r="B58" s="151"/>
-      <c r="C58" s="154"/>
-      <c r="D58" s="151"/>
-      <c r="E58" s="151"/>
-      <c r="F58" s="151"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="151"/>
-      <c r="B59" s="151"/>
-      <c r="C59" s="154"/>
-      <c r="D59" s="151"/>
-      <c r="E59" s="151"/>
-      <c r="F59" s="151"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="151"/>
-      <c r="B60" s="151"/>
-      <c r="C60" s="154"/>
-      <c r="D60" s="151"/>
-      <c r="E60" s="151"/>
-      <c r="F60" s="151"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="151"/>
-      <c r="B61" s="151"/>
-      <c r="C61" s="154"/>
-      <c r="D61" s="151"/>
-      <c r="E61" s="151"/>
-      <c r="F61" s="151"/>
+      <c r="A16" s="151" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" s="151">
+        <v>50</v>
+      </c>
+      <c r="C16" s="154">
+        <v>42900</v>
+      </c>
+      <c r="D16" s="151" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="151">
+        <v>60185230</v>
+      </c>
+      <c r="F16" s="151">
+        <v>376</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>CONSTITUCION</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>228</v>
+      </c>
+      <c r="B17">
+        <v>38</v>
+      </c>
+      <c r="C17" s="38">
+        <v>39940</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17">
+        <v>402087</v>
+      </c>
+      <c r="F17" s="151">
+        <v>47</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>CONSTITUCION</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>228</v>
+      </c>
+      <c r="B18">
+        <v>80</v>
+      </c>
+      <c r="C18" s="38">
+        <v>41547</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18">
+        <v>4321139</v>
+      </c>
+      <c r="F18" s="151">
+        <v>1226</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>CONSTITUCION</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="151" t="s">
+        <v>205</v>
+      </c>
+      <c r="B19" s="151">
+        <v>38</v>
+      </c>
+      <c r="C19" s="154">
+        <v>42227</v>
+      </c>
+      <c r="D19" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="151">
+        <v>343196</v>
+      </c>
+      <c r="F19" s="151">
+        <v>50</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>CURANIPE</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="151" t="s">
+        <v>205</v>
+      </c>
+      <c r="B20" s="151">
+        <v>38</v>
+      </c>
+      <c r="C20" s="154">
+        <v>37278</v>
+      </c>
+      <c r="D20" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="151">
+        <v>1301286</v>
+      </c>
+      <c r="F20" s="151">
+        <v>70</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>CURANIPE</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="151" t="s">
+        <v>205</v>
+      </c>
+      <c r="B21" s="151">
+        <v>38</v>
+      </c>
+      <c r="C21" s="154">
+        <v>43703</v>
+      </c>
+      <c r="D21" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="151">
+        <v>343112</v>
+      </c>
+      <c r="F21" s="151">
+        <v>25</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>CURANIPE</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="151" t="s">
+        <v>205</v>
+      </c>
+      <c r="B22" s="151">
+        <v>50</v>
+      </c>
+      <c r="C22" s="154">
+        <v>41933</v>
+      </c>
+      <c r="D22" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="151">
+        <v>345478</v>
+      </c>
+      <c r="F22" s="151">
+        <v>20</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>CURANIPE</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="151" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="151">
+        <v>19</v>
+      </c>
+      <c r="C23" s="154">
+        <v>42366</v>
+      </c>
+      <c r="D23" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="151">
+        <v>60146168</v>
+      </c>
+      <c r="F23" s="151">
+        <v>25</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>CURICO</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="151" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="151">
+        <v>19</v>
+      </c>
+      <c r="C24" s="154">
+        <v>37279</v>
+      </c>
+      <c r="D24" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="151">
+        <v>1390704</v>
+      </c>
+      <c r="F24" s="151">
+        <v>14</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>CURICO</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="151" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="151">
+        <v>19</v>
+      </c>
+      <c r="C25" s="154">
+        <v>39412</v>
+      </c>
+      <c r="D25" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="151">
+        <v>4625688</v>
+      </c>
+      <c r="F25" s="151">
+        <v>5</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>CURICO</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="151" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" s="151">
+        <v>13</v>
+      </c>
+      <c r="C26" s="154">
+        <v>44252</v>
+      </c>
+      <c r="D26" s="151" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="151">
+        <v>584227</v>
+      </c>
+      <c r="F26" s="151">
+        <v>7</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>CURICO</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="151" t="s">
+        <v>128</v>
+      </c>
+      <c r="B27" s="151">
+        <v>19</v>
+      </c>
+      <c r="C27" s="154">
+        <v>40008</v>
+      </c>
+      <c r="D27" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="151">
+        <v>371308</v>
+      </c>
+      <c r="F27" s="151">
+        <v>4</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>CURICO</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="151" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="151">
+        <v>19</v>
+      </c>
+      <c r="C28" s="154">
+        <v>39244</v>
+      </c>
+      <c r="D28" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="151">
+        <v>1320102</v>
+      </c>
+      <c r="F28" s="151">
+        <v>13</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>CURICO</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="151" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="151">
+        <v>13</v>
+      </c>
+      <c r="C29" s="154">
+        <v>40358</v>
+      </c>
+      <c r="D29" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="151">
+        <v>536655</v>
+      </c>
+      <c r="F29" s="151">
+        <v>11</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>CURICO</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="151" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="151">
+        <v>13</v>
+      </c>
+      <c r="C30" s="154">
+        <v>37769</v>
+      </c>
+      <c r="D30" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="151">
+        <v>1446368</v>
+      </c>
+      <c r="F30" s="151">
+        <v>22</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>CURICO</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="151" t="s">
+        <v>128</v>
+      </c>
+      <c r="B31" s="151">
+        <v>19</v>
+      </c>
+      <c r="C31" s="154">
+        <v>42142</v>
+      </c>
+      <c r="D31" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="151">
+        <v>60129823</v>
+      </c>
+      <c r="F31" s="151">
+        <v>3</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>CURICO</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="151" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="151">
+        <v>19</v>
+      </c>
+      <c r="C32" s="154">
+        <v>43936</v>
+      </c>
+      <c r="D32" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="151">
+        <v>60256447</v>
+      </c>
+      <c r="F32" s="151">
+        <v>7</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>LINARES</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="151" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="151">
+        <v>13</v>
+      </c>
+      <c r="C33" s="154">
+        <v>44463</v>
+      </c>
+      <c r="D33" s="151" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="151">
+        <v>1366785</v>
+      </c>
+      <c r="F33" s="151">
+        <v>8</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>LINARES</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="151" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="151">
+        <v>19</v>
+      </c>
+      <c r="C34" s="154">
+        <v>38762</v>
+      </c>
+      <c r="D34" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="151">
+        <v>4273798</v>
+      </c>
+      <c r="F34" s="151">
+        <v>23</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>LINARES</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="151" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" s="151">
+        <v>19</v>
+      </c>
+      <c r="C35" s="154">
+        <v>37488</v>
+      </c>
+      <c r="D35" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" s="151">
+        <v>1415904</v>
+      </c>
+      <c r="F35" s="151">
+        <v>7</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>LINARES</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="151" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="151">
+        <v>13</v>
+      </c>
+      <c r="C36" s="154">
+        <v>39531</v>
+      </c>
+      <c r="D36" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="151">
+        <v>4663376</v>
+      </c>
+      <c r="F36" s="151">
+        <v>11</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>LINARES</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="151" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="151">
+        <v>13</v>
+      </c>
+      <c r="C37" s="154">
+        <v>37588</v>
+      </c>
+      <c r="D37" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="151">
+        <v>442022</v>
+      </c>
+      <c r="F37" s="151">
+        <v>11</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>LINARES</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="151" t="s">
+        <v>241</v>
+      </c>
+      <c r="B38" s="151">
+        <v>19</v>
+      </c>
+      <c r="C38" s="154">
+        <v>43171</v>
+      </c>
+      <c r="D38" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="151">
+        <v>60202327</v>
+      </c>
+      <c r="F38" s="151">
+        <v>13</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>LONGAVI</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="151" t="s">
+        <v>241</v>
+      </c>
+      <c r="B39" s="151">
+        <v>19</v>
+      </c>
+      <c r="C39" s="154">
+        <v>43171</v>
+      </c>
+      <c r="D39" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="151">
+        <v>60202278</v>
+      </c>
+      <c r="F39" s="151">
+        <v>15</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>LONGAVI</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="151" t="s">
+        <v>215</v>
+      </c>
+      <c r="B40" s="151">
+        <v>38</v>
+      </c>
+      <c r="C40" s="154">
+        <v>41699</v>
+      </c>
+      <c r="D40" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="151">
+        <v>4969794</v>
+      </c>
+      <c r="F40" s="151">
+        <v>26</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>PELLUHUE</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="151" t="s">
+        <v>215</v>
+      </c>
+      <c r="B41" s="151">
+        <v>38</v>
+      </c>
+      <c r="C41" s="154">
+        <v>42131</v>
+      </c>
+      <c r="D41" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="151">
+        <v>60127153</v>
+      </c>
+      <c r="F41" s="151">
+        <v>101</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>PELLUHUE</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="151" t="s">
+        <v>259</v>
+      </c>
+      <c r="B42" s="151">
+        <v>13</v>
+      </c>
+      <c r="C42" s="154">
+        <v>39639</v>
+      </c>
+      <c r="D42" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="151">
+        <v>1167467</v>
+      </c>
+      <c r="F42" s="151">
+        <v>1</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>SAN JAVIER</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="151" t="s">
+        <v>259</v>
+      </c>
+      <c r="B43" s="151">
+        <v>19</v>
+      </c>
+      <c r="C43" s="154">
+        <v>44097</v>
+      </c>
+      <c r="D43" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="151">
+        <v>60268415</v>
+      </c>
+      <c r="F43" s="151">
+        <v>11</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v>SAN JAVIER</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" s="151">
+        <v>13</v>
+      </c>
+      <c r="C44" s="154">
+        <v>40424</v>
+      </c>
+      <c r="D44" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="151">
+        <v>993685</v>
+      </c>
+      <c r="F44" s="151">
+        <v>12</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" s="151">
+        <v>13</v>
+      </c>
+      <c r="C45" s="154">
+        <v>40284</v>
+      </c>
+      <c r="D45" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="151">
+        <v>47222</v>
+      </c>
+      <c r="F45" s="151">
+        <v>15</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B46" s="151">
+        <v>19</v>
+      </c>
+      <c r="C46" s="154">
+        <v>37443</v>
+      </c>
+      <c r="D46" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="151">
+        <v>144501</v>
+      </c>
+      <c r="F46" s="151">
+        <v>49</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" s="151">
+        <v>13</v>
+      </c>
+      <c r="C47" s="154">
+        <v>40121</v>
+      </c>
+      <c r="D47" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="151">
+        <v>666708</v>
+      </c>
+      <c r="F47" s="151">
+        <v>5</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" s="151">
+        <v>13</v>
+      </c>
+      <c r="C48" s="154">
+        <v>41751</v>
+      </c>
+      <c r="D48" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="151">
+        <v>950985</v>
+      </c>
+      <c r="F48" s="151">
+        <v>32</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="151">
+        <v>13</v>
+      </c>
+      <c r="C49" s="154">
+        <v>44302</v>
+      </c>
+      <c r="D49" s="151" t="s">
+        <v>29</v>
+      </c>
+      <c r="E49" s="151">
+        <v>1351105</v>
+      </c>
+      <c r="F49" s="151">
+        <v>14</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B50" s="151">
+        <v>19</v>
+      </c>
+      <c r="C50" s="154">
+        <v>42822</v>
+      </c>
+      <c r="D50" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="151">
+        <v>60182454</v>
+      </c>
+      <c r="F50" s="151">
+        <v>11</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" s="151">
+        <v>25</v>
+      </c>
+      <c r="C51" s="154">
+        <v>37497</v>
+      </c>
+      <c r="D51" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="151">
+        <v>1418480</v>
+      </c>
+      <c r="F51" s="151">
+        <v>19</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" s="151">
+        <v>19</v>
+      </c>
+      <c r="C52" s="154">
+        <v>40305</v>
+      </c>
+      <c r="D52" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="151">
+        <v>5044456</v>
+      </c>
+      <c r="F52" s="151">
+        <v>2</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B53" s="151">
+        <v>13</v>
+      </c>
+      <c r="C53" s="154">
+        <v>40085</v>
+      </c>
+      <c r="D53" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" s="151">
+        <v>1000251</v>
+      </c>
+      <c r="F53" s="151">
+        <v>8</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B54" s="151">
+        <v>19</v>
+      </c>
+      <c r="C54" s="154">
+        <v>36853</v>
+      </c>
+      <c r="D54" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="151">
+        <v>255430</v>
+      </c>
+      <c r="F54" s="151">
+        <v>18</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" s="151">
+        <v>19</v>
+      </c>
+      <c r="C55" s="154">
+        <v>38280</v>
+      </c>
+      <c r="D55" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="151">
+        <v>4084658</v>
+      </c>
+      <c r="F55" s="151">
+        <v>3</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B56" s="151">
+        <v>25</v>
+      </c>
+      <c r="C56" s="154">
+        <v>41369</v>
+      </c>
+      <c r="D56" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" s="151">
+        <v>60055953</v>
+      </c>
+      <c r="F56" s="151">
+        <v>17</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" s="151">
+        <v>19</v>
+      </c>
+      <c r="C57" s="154">
+        <v>38673</v>
+      </c>
+      <c r="D57" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="151">
+        <v>845817</v>
+      </c>
+      <c r="F57" s="151">
+        <v>8</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B58" s="151">
+        <v>13</v>
+      </c>
+      <c r="C58" s="154">
+        <v>40205</v>
+      </c>
+      <c r="D58" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" s="151">
+        <v>1201396</v>
+      </c>
+      <c r="F58" s="151">
+        <v>7</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B59" s="151">
+        <v>13</v>
+      </c>
+      <c r="C59" s="154">
+        <v>40192</v>
+      </c>
+      <c r="D59" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="151">
+        <v>38157</v>
+      </c>
+      <c r="F59" s="151">
+        <v>10</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B60" s="151">
+        <v>19</v>
+      </c>
+      <c r="C60" s="154">
+        <v>40305</v>
+      </c>
+      <c r="D60" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="151">
+        <v>5040669</v>
+      </c>
+      <c r="F60" s="151">
+        <v>17</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" s="151">
+        <v>19</v>
+      </c>
+      <c r="C61" s="154">
+        <v>43910</v>
+      </c>
+      <c r="D61" s="151" t="s">
+        <v>31</v>
+      </c>
+      <c r="E61" s="151">
+        <v>1294160</v>
+      </c>
+      <c r="F61" s="151">
+        <v>14</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="0"/>
+        <v>TALCA</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G61" xr:uid="{05F3A346-95CC-40C7-A048-A8DCA15A773E}">
@@ -28302,14 +29876,17 @@
       <sortCondition ref="A1:A26"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="E2:E16 E20:E6692">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="E2:E16 E20:E61">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62:E6692">
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6693:E20621">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20622:E26969">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28319,8 +29896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3D49A9-06A7-46DC-9EBC-1914E499D5E6}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
separar la lógica funcionando tambien en IyF, listo para entrega
</commit_message>
<xml_diff>
--- a/Code/Limpio/Excels/modelo MM - TALCA 28.12_v6.xlsx
+++ b/Code/Limpio/Excels/modelo MM - TALCA 28.12_v6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\6020.Inecon_ModeloVanMedicion\6020.Inecon_ModeloVanMedicion\Code\Limpio\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918D23C9-5D7A-4A4D-AE46-34884BA73132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B79B0E-8362-45CB-970A-29F31FAC9DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="834" firstSheet="7" activeTab="13" xr2:uid="{0B67A8E0-BE2B-4F48-8F89-95A6B35879D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="834" activeTab="2" xr2:uid="{0B67A8E0-BE2B-4F48-8F89-95A6B35879D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos_Tarifas" sheetId="13" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="355">
   <si>
     <t>Intervalo (l/h)</t>
   </si>
@@ -1677,7 +1677,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="173" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2031,6 +2031,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -7256,8 +7259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CBA8B56-86C0-48DC-8876-01FB76341A5D}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7338,9 +7341,8 @@
       <c r="C5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="D5" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -7350,12 +7352,11 @@
       <c r="B6" s="31">
         <v>50</v>
       </c>
-      <c r="C6" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="C6" s="161" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -7413,9 +7414,8 @@
       <c r="C10" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="D10" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -7428,9 +7428,8 @@
       <c r="C11" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="D11" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -7440,12 +7439,11 @@
       <c r="B12" s="31">
         <v>50</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="C12" s="161" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -7455,12 +7453,11 @@
       <c r="B13" s="31">
         <v>75</v>
       </c>
-      <c r="C13" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="C13" s="161" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -7470,12 +7467,11 @@
       <c r="B14" s="31">
         <v>80</v>
       </c>
-      <c r="C14" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="C14" s="161" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -7485,12 +7481,11 @@
       <c r="B15" s="31">
         <v>100</v>
       </c>
-      <c r="C15" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="C15" s="161" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -7548,9 +7543,8 @@
       <c r="C19" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="D19" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -7560,12 +7554,11 @@
       <c r="B20" s="31">
         <v>50</v>
       </c>
-      <c r="C20" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="C20" s="161" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -7575,12 +7568,11 @@
       <c r="B21" s="31">
         <v>80</v>
       </c>
-      <c r="C21" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="C21" s="161" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -7638,9 +7630,8 @@
       <c r="C25" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="D25" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -7695,12 +7686,11 @@
       <c r="B29" s="31">
         <v>50</v>
       </c>
-      <c r="C29" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="C29" s="161" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -7710,12 +7700,11 @@
       <c r="B30" s="31">
         <v>80</v>
       </c>
-      <c r="C30" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v>ULTRA</v>
+      <c r="C30" s="161" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="161" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -11728,7 +11717,7 @@
       <c r="V98" s="75"/>
     </row>
     <row r="99" spans="1:22" s="76" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="161" t="s">
+      <c r="B99" s="162" t="s">
         <v>165</v>
       </c>
       <c r="C99" s="77" t="s">
@@ -11755,7 +11744,7 @@
       <c r="S99" s="78"/>
     </row>
     <row r="100" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B100" s="162"/>
+      <c r="B100" s="163"/>
       <c r="C100" s="79"/>
       <c r="D100" s="80"/>
       <c r="E100" s="80"/>
@@ -11775,7 +11764,7 @@
       <c r="S100" s="80"/>
     </row>
     <row r="101" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B101" s="162"/>
+      <c r="B101" s="163"/>
       <c r="C101" s="76" t="s">
         <v>167</v>
       </c>
@@ -11800,7 +11789,7 @@
       <c r="S101" s="80"/>
     </row>
     <row r="102" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B102" s="162"/>
+      <c r="B102" s="163"/>
       <c r="D102" s="81"/>
       <c r="E102" s="81"/>
       <c r="F102" s="81"/>
@@ -11819,7 +11808,7 @@
       <c r="S102" s="81"/>
     </row>
     <row r="103" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B103" s="162"/>
+      <c r="B103" s="163"/>
       <c r="D103" s="81"/>
       <c r="E103" s="81"/>
       <c r="F103" s="81"/>
@@ -11838,7 +11827,7 @@
       <c r="S103" s="81"/>
     </row>
     <row r="104" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B104" s="162"/>
+      <c r="B104" s="163"/>
       <c r="C104" s="79" t="s">
         <v>168</v>
       </c>
@@ -11909,7 +11898,7 @@
       <c r="A105" s="76">
         <v>1</v>
       </c>
-      <c r="B105" s="162"/>
+      <c r="B105" s="163"/>
       <c r="C105" s="76" t="s">
         <v>169</v>
       </c>
@@ -11977,7 +11966,7 @@
       <c r="U105" s="82"/>
     </row>
     <row r="106" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B106" s="162"/>
+      <c r="B106" s="163"/>
       <c r="C106" s="83"/>
       <c r="D106" s="84"/>
       <c r="E106" s="85"/>
@@ -11997,7 +11986,7 @@
       <c r="S106" s="85"/>
     </row>
     <row r="107" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B107" s="162"/>
+      <c r="B107" s="163"/>
       <c r="C107" s="76" t="s">
         <v>170</v>
       </c>
@@ -12019,7 +12008,7 @@
       <c r="S107" s="81"/>
     </row>
     <row r="108" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B108" s="162"/>
+      <c r="B108" s="163"/>
       <c r="C108" s="86" t="s">
         <v>171</v>
       </c>
@@ -12045,7 +12034,7 @@
       <c r="T108" s="87"/>
     </row>
     <row r="109" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B109" s="162"/>
+      <c r="B109" s="163"/>
       <c r="C109" s="86" t="s">
         <v>172</v>
       </c>
@@ -12116,7 +12105,7 @@
       <c r="A110" s="76">
         <v>10</v>
       </c>
-      <c r="B110" s="162"/>
+      <c r="B110" s="163"/>
       <c r="C110" s="86" t="s">
         <v>173</v>
       </c>
@@ -12186,7 +12175,7 @@
       <c r="A111" s="88">
         <v>0.27</v>
       </c>
-      <c r="B111" s="163"/>
+      <c r="B111" s="164"/>
       <c r="C111" s="89" t="s">
         <v>174</v>
       </c>
@@ -14799,8 +14788,8 @@
   </sheetPr>
   <dimension ref="A3:V182"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -15553,16 +15542,13 @@
         <v>5.5754722615727106</v>
       </c>
       <c r="H26" s="58">
-        <f t="shared" si="5"/>
-        <v>17.012046100830631</v>
+        <v>16.612046100000001</v>
       </c>
       <c r="I26" s="58">
-        <f t="shared" si="5"/>
-        <v>26.496398281819843</v>
+        <v>26.096398279999999</v>
       </c>
       <c r="J26" s="58">
-        <f t="shared" si="5"/>
-        <v>32.762679783922579</v>
+        <v>32.362679780000001</v>
       </c>
       <c r="K26" s="58">
         <f t="shared" si="5"/>
@@ -15655,6 +15641,15 @@
       </c>
       <c r="F34" s="44" t="s">
         <v>154</v>
+      </c>
+      <c r="J34" s="44">
+        <v>17.012046100830631</v>
+      </c>
+      <c r="K34" s="44">
+        <v>26.496398281819843</v>
+      </c>
+      <c r="L34" s="44">
+        <v>32.762679783922579</v>
       </c>
     </row>
     <row r="37" spans="2:19" hidden="1" x14ac:dyDescent="0.3">
@@ -18196,7 +18191,7 @@
       <c r="V99" s="75"/>
     </row>
     <row r="100" spans="1:22" s="76" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="161" t="s">
+      <c r="B100" s="162" t="s">
         <v>165</v>
       </c>
       <c r="C100" s="77" t="s">
@@ -18223,7 +18218,7 @@
       <c r="S100" s="78"/>
     </row>
     <row r="101" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B101" s="162"/>
+      <c r="B101" s="163"/>
       <c r="C101" s="79"/>
       <c r="D101" s="80"/>
       <c r="E101" s="80"/>
@@ -18243,7 +18238,7 @@
       <c r="S101" s="80"/>
     </row>
     <row r="102" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B102" s="162"/>
+      <c r="B102" s="163"/>
       <c r="C102" s="76" t="s">
         <v>167</v>
       </c>
@@ -18268,7 +18263,7 @@
       <c r="S102" s="80"/>
     </row>
     <row r="103" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B103" s="162"/>
+      <c r="B103" s="163"/>
       <c r="D103" s="81"/>
       <c r="E103" s="81"/>
       <c r="F103" s="81"/>
@@ -18287,7 +18282,7 @@
       <c r="S103" s="81"/>
     </row>
     <row r="104" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B104" s="162"/>
+      <c r="B104" s="163"/>
       <c r="D104" s="81"/>
       <c r="E104" s="81"/>
       <c r="F104" s="81"/>
@@ -18306,7 +18301,7 @@
       <c r="S104" s="81"/>
     </row>
     <row r="105" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B105" s="162"/>
+      <c r="B105" s="163"/>
       <c r="C105" s="79" t="s">
         <v>168</v>
       </c>
@@ -18377,7 +18372,7 @@
       <c r="A106" s="76">
         <v>1</v>
       </c>
-      <c r="B106" s="162"/>
+      <c r="B106" s="163"/>
       <c r="C106" s="76" t="s">
         <v>169</v>
       </c>
@@ -18445,7 +18440,7 @@
       <c r="U106" s="82"/>
     </row>
     <row r="107" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B107" s="162"/>
+      <c r="B107" s="163"/>
       <c r="C107" s="83"/>
       <c r="D107" s="84"/>
       <c r="E107" s="85"/>
@@ -18465,7 +18460,7 @@
       <c r="S107" s="85"/>
     </row>
     <row r="108" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B108" s="162"/>
+      <c r="B108" s="163"/>
       <c r="C108" s="76" t="s">
         <v>170</v>
       </c>
@@ -18487,7 +18482,7 @@
       <c r="S108" s="81"/>
     </row>
     <row r="109" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B109" s="162"/>
+      <c r="B109" s="163"/>
       <c r="C109" s="86" t="s">
         <v>171</v>
       </c>
@@ -18513,7 +18508,7 @@
       <c r="T109" s="87"/>
     </row>
     <row r="110" spans="1:22" s="76" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B110" s="162"/>
+      <c r="B110" s="163"/>
       <c r="C110" s="86" t="s">
         <v>172</v>
       </c>
@@ -18584,7 +18579,7 @@
       <c r="A111" s="76">
         <v>10</v>
       </c>
-      <c r="B111" s="162"/>
+      <c r="B111" s="163"/>
       <c r="C111" s="86" t="s">
         <v>173</v>
       </c>
@@ -18654,7 +18649,7 @@
       <c r="A112" s="88">
         <v>0.27</v>
       </c>
-      <c r="B112" s="163"/>
+      <c r="B112" s="164"/>
       <c r="C112" s="89" t="s">
         <v>174</v>
       </c>
@@ -22480,7 +22475,7 @@
       <c r="V50" s="75"/>
     </row>
     <row r="51" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="161" t="s">
+      <c r="B51" s="162" t="s">
         <v>165</v>
       </c>
       <c r="C51" s="77" t="s">
@@ -22538,7 +22533,7 @@
       </c>
     </row>
     <row r="52" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="162"/>
+      <c r="B52" s="163"/>
       <c r="C52" s="79"/>
       <c r="D52" s="80"/>
       <c r="E52" s="80"/>
@@ -22558,7 +22553,7 @@
       <c r="S52" s="80"/>
     </row>
     <row r="53" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="162"/>
+      <c r="B53" s="163"/>
       <c r="C53" s="76" t="s">
         <v>167</v>
       </c>
@@ -22580,7 +22575,7 @@
       <c r="S53" s="80"/>
     </row>
     <row r="54" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="162"/>
+      <c r="B54" s="163"/>
       <c r="D54" s="81"/>
       <c r="E54" s="81"/>
       <c r="F54" s="81"/>
@@ -22599,7 +22594,7 @@
       <c r="S54" s="81"/>
     </row>
     <row r="55" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="162"/>
+      <c r="B55" s="163"/>
       <c r="D55" s="81"/>
       <c r="E55" s="81"/>
       <c r="F55" s="81"/>
@@ -22618,7 +22613,7 @@
       <c r="S55" s="81"/>
     </row>
     <row r="56" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="162"/>
+      <c r="B56" s="163"/>
       <c r="C56" s="79" t="s">
         <v>168</v>
       </c>
@@ -22688,7 +22683,7 @@
       <c r="A57" s="76">
         <v>1</v>
       </c>
-      <c r="B57" s="162"/>
+      <c r="B57" s="163"/>
       <c r="C57" s="76" t="s">
         <v>169</v>
       </c>
@@ -22755,7 +22750,7 @@
       </c>
     </row>
     <row r="58" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="162"/>
+      <c r="B58" s="163"/>
       <c r="C58" s="83"/>
       <c r="D58" s="84"/>
       <c r="E58" s="85"/>
@@ -22775,7 +22770,7 @@
       <c r="S58" s="85"/>
     </row>
     <row r="59" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="162"/>
+      <c r="B59" s="163"/>
       <c r="C59" s="76" t="s">
         <v>170</v>
       </c>
@@ -22797,7 +22792,7 @@
       <c r="S59" s="81"/>
     </row>
     <row r="60" spans="1:22" s="76" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="162"/>
+      <c r="B60" s="163"/>
       <c r="C60" s="86" t="s">
         <v>171</v>
       </c>
@@ -22825,7 +22820,7 @@
       <c r="A61" s="76">
         <v>10</v>
       </c>
-      <c r="B61" s="162"/>
+      <c r="B61" s="163"/>
       <c r="C61" s="86" t="s">
         <v>173</v>
       </c>
@@ -22895,7 +22890,7 @@
       <c r="A62" s="88">
         <v>0.27</v>
       </c>
-      <c r="B62" s="163"/>
+      <c r="B62" s="164"/>
       <c r="C62" s="89" t="s">
         <v>174</v>
       </c>
@@ -25336,7 +25331,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25375,7 +25370,7 @@
         <v>347</v>
       </c>
       <c r="C3" s="153">
-        <v>0.65</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -25397,7 +25392,7 @@
         <v>348</v>
       </c>
       <c r="C5">
-        <v>600000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -30519,11 +30514,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="afef9374-bd24-49fe-b5be-cd056ccbd7a9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -30715,26 +30711,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="afef9374-bd24-49fe-b5be-cd056ccbd7a9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F368767-011F-4603-B6D3-67B09FEB0E3E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{799D9F8D-2034-4116-9680-A411761E28F5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="afef9374-bd24-49fe-b5be-cd056ccbd7a9"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -30758,9 +30745,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{799D9F8D-2034-4116-9680-A411761E28F5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F368767-011F-4603-B6D3-67B09FEB0E3E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="afef9374-bd24-49fe-b5be-cd056ccbd7a9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>